<commit_message>
Fixed checkmarks, ran on ass00 and ass03
</commit_message>
<xml_diff>
--- a/S2022_Tests/ASS_00_Dim_Testing/StudentFolder/Ex.1/ExcelExtract.xlsx
+++ b/S2022_Tests/ASS_00_Dim_Testing/StudentFolder/Ex.1/ExcelExtract.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zacha\OneDrive\Desktop\Ualberta Summer 2022 Co-op\SolidWorks\AutoMARK\AutoMARK_V6\S2022_Tests\ASS_00_Dim_Testing\StudentFolder\Ex.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{956A140B-F008-47A4-B41E-64453687DE59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0515821C-738A-4DB3-88F7-71765D77CF24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="953" yWindow="2847" windowWidth="13120" windowHeight="7660" xr2:uid="{49E7E77B-33C7-41D0-ABBD-B77019454604}"/>
+    <workbookView xWindow="953" yWindow="2847" windowWidth="13120" windowHeight="7660" xr2:uid="{4C7DEA34-2B3B-428A-9145-4FF74F126DC4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1406,7 +1406,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A01C9D0E-4E5C-4262-B3BE-B6B40C233587}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D74765D-8019-40A1-ABDA-2DD9A406A1E1}">
   <dimension ref="A1:AS125"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -6619,13 +6619,13 @@
         <v>0</v>
       </c>
       <c r="AP74">
-        <v>4.5280113207547074E-2</v>
+        <v>4.5280113207547115E-2</v>
       </c>
       <c r="AQ74">
         <v>0.13875716981132069</v>
       </c>
       <c r="AR74">
-        <v>4.5280113207547074E-2</v>
+        <v>4.5280113207547115E-2</v>
       </c>
       <c r="AS74">
         <v>0.10125716981132069</v>
@@ -6732,13 +6732,13 @@
         <v>0</v>
       </c>
       <c r="AP75">
-        <v>3.3280113207547063E-2</v>
+        <v>3.3280113207547105E-2</v>
       </c>
       <c r="AQ75">
         <v>0.1512571698113207</v>
       </c>
       <c r="AR75">
-        <v>3.3280113207547063E-2</v>
+        <v>3.3280113207547105E-2</v>
       </c>
       <c r="AS75">
         <v>0.10125716981132069</v>
@@ -6958,16 +6958,16 @@
         <v>0</v>
       </c>
       <c r="AP77">
-        <v>0.19568968234456149</v>
+        <v>0.19568968234456152</v>
       </c>
       <c r="AQ77">
         <v>0.10125716981132069</v>
       </c>
       <c r="AR77">
-        <v>0.16255547525085495</v>
+        <v>0.16255547525085492</v>
       </c>
       <c r="AS77">
-        <v>0.11498180776801278</v>
+        <v>0.11498180776801281</v>
       </c>
     </row>
     <row r="78" spans="1:45" s="4" customFormat="1" x14ac:dyDescent="0.5">
@@ -7703,13 +7703,13 @@
         <v>0.17378011320754708</v>
       </c>
       <c r="AQ88">
-        <v>0.25113373584905668</v>
+        <v>0.25113373584905663</v>
       </c>
       <c r="AR88">
         <v>6.1280113207547067E-2</v>
       </c>
       <c r="AS88">
-        <v>0.25113373584905657</v>
+        <v>0.25113373584905652</v>
       </c>
     </row>
     <row r="89" spans="1:45" x14ac:dyDescent="0.5">
@@ -7819,16 +7819,16 @@
         <v>0</v>
       </c>
       <c r="AP89">
-        <v>8.5442771981199872E-2</v>
+        <v>8.5442771981199886E-2</v>
       </c>
       <c r="AQ89">
-        <v>0.20125873584905662</v>
+        <v>0.2012587358490566</v>
       </c>
       <c r="AR89">
-        <v>7.4617454433894337E-2</v>
+        <v>7.4617454433894351E-2</v>
       </c>
       <c r="AS89">
-        <v>0.20750873584905655</v>
+        <v>0.20750873584905652</v>
       </c>
     </row>
     <row r="90" spans="1:45" x14ac:dyDescent="0.5">
@@ -7938,13 +7938,13 @@
         <v>0</v>
       </c>
       <c r="AP90">
-        <v>8.9689371470437804E-2</v>
+        <v>8.9689371470437818E-2</v>
       </c>
       <c r="AQ90">
         <v>0.20697192630008165</v>
       </c>
       <c r="AR90">
-        <v>7.0370854944656405E-2</v>
+        <v>7.0370854944656419E-2</v>
       </c>
       <c r="AS90">
         <v>0.20179554539803135</v>
@@ -8057,7 +8057,7 @@
         <v>0</v>
       </c>
       <c r="AP91">
-        <v>8.8535242464194308E-2</v>
+        <v>8.8535242464194336E-2</v>
       </c>
       <c r="AQ91">
         <v>0.21354412756162663</v>
@@ -8182,13 +8182,13 @@
         <v>0</v>
       </c>
       <c r="AP92">
-        <v>0.11253011320754711</v>
+        <v>0.11253011320754709</v>
       </c>
       <c r="AQ92">
         <v>0.2130439898869009</v>
       </c>
       <c r="AR92">
-        <v>0.12253011320754706</v>
+        <v>0.12253011320754705</v>
       </c>
       <c r="AS92">
         <v>0.1957234818112121</v>
@@ -8301,13 +8301,13 @@
         <v>0</v>
       </c>
       <c r="AP93">
-        <v>0.1249875556434544</v>
+        <v>0.12498755564345439</v>
       </c>
       <c r="AQ93">
         <v>0.21441551297552461</v>
       </c>
       <c r="AR93">
-        <v>0.11007267077163976</v>
+        <v>0.11007267077163975</v>
       </c>
       <c r="AS93">
         <v>0.1943519587225884</v>
@@ -8417,13 +8417,13 @@
         <v>8.0030113207547104E-2</v>
       </c>
       <c r="AQ94">
-        <v>0.23913373584905637</v>
+        <v>0.23913373584905634</v>
       </c>
       <c r="AR94">
         <v>6.1280113207547102E-2</v>
       </c>
       <c r="AS94">
-        <v>0.23913373584905637</v>
+        <v>0.23913373584905634</v>
       </c>
     </row>
     <row r="95" spans="1:45" x14ac:dyDescent="0.5">
@@ -8530,13 +8530,13 @@
         <v>8.0030113207547104E-2</v>
       </c>
       <c r="AQ95">
-        <v>0.23913373584905656</v>
+        <v>0.23913373584905651</v>
       </c>
       <c r="AR95">
         <v>0.1175301132075471</v>
       </c>
       <c r="AS95">
-        <v>0.23913373584905656</v>
+        <v>0.23913373584905651</v>
       </c>
     </row>
     <row r="96" spans="1:45" x14ac:dyDescent="0.5">
@@ -9481,13 +9481,13 @@
         <v>0.21676071698113181</v>
       </c>
       <c r="AQ107">
-        <v>0.1764790448157911</v>
+        <v>0.17647904481579105</v>
       </c>
       <c r="AR107">
         <v>0.25426071698113184</v>
       </c>
       <c r="AS107">
-        <v>0.1764790448157911</v>
+        <v>0.17647904481579105</v>
       </c>
     </row>
     <row r="108" spans="1:45" s="4" customFormat="1" x14ac:dyDescent="0.5">
@@ -10471,10 +10471,10 @@
         <v>0</v>
       </c>
       <c r="AP119">
-        <v>0.34185913666902662</v>
+        <v>0.34185913666902673</v>
       </c>
       <c r="AQ119">
-        <v>0.13499630084857919</v>
+        <v>0.13499630084857916</v>
       </c>
       <c r="AR119">
         <v>0</v>
@@ -10759,10 +10759,10 @@
         <v>2</v>
       </c>
       <c r="O125">
-        <v>0.30460033668052133</v>
+        <v>0.30442814140648361</v>
       </c>
       <c r="P125">
-        <v>7.6355819300822123E-2</v>
+        <v>7.616736879291526E-2</v>
       </c>
       <c r="Q125">
         <v>0.28439264478139581</v>

</xml_diff>

<commit_message>
Saved file location when clicking on various buttons
</commit_message>
<xml_diff>
--- a/S2022_Tests/ASS_00_Dim_Testing/StudentFolder/Ex.1/ExcelExtract.xlsx
+++ b/S2022_Tests/ASS_00_Dim_Testing/StudentFolder/Ex.1/ExcelExtract.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zacha\OneDrive\Desktop\Ualberta Summer 2022 Co-op\SolidWorks\AutoMARK\AutoMARK_V6\S2022_Tests\ASS_00_Dim_Testing\StudentFolder\Ex.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{26D58E23-1768-48A5-A211-76201B36823E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6FA1F345-FB27-4F85-9023-B3989CE33F56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="953" yWindow="2847" windowWidth="13120" windowHeight="7660" xr2:uid="{15C94D8E-89EC-496A-945A-D0453465050E}"/>
+    <workbookView xWindow="3247" yWindow="327" windowWidth="7513" windowHeight="7800" xr2:uid="{6AFA57C4-F4E6-4ECD-9039-D68C5DF33D11}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1406,7 +1406,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F6F223B-050E-41D0-B263-950A053870C6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1F0270E-78F4-440C-92B7-47AD31428F28}">
   <dimension ref="A1:AS125"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Fixed chamfer, now accepts lesser of angle or 180-angle
</commit_message>
<xml_diff>
--- a/S2022_Tests/ASS_00_Dim_Testing/StudentFolder/Ex.1/ExcelExtract.xlsx
+++ b/S2022_Tests/ASS_00_Dim_Testing/StudentFolder/Ex.1/ExcelExtract.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zacha\OneDrive\Desktop\Ualberta Summer 2022 Co-op\SolidWorks\AutoMARK\AutoMARK_V6\S2022_Tests\ASS_00_Dim_Testing\StudentFolder\Ex.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6FA1F345-FB27-4F85-9023-B3989CE33F56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{512A9BA3-735D-4429-A952-4058048799A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3247" yWindow="327" windowWidth="7513" windowHeight="7800" xr2:uid="{6AFA57C4-F4E6-4ECD-9039-D68C5DF33D11}"/>
+    <workbookView xWindow="3587" yWindow="667" windowWidth="7513" windowHeight="7800" xr2:uid="{ED4BFFBB-1C68-443E-ACC6-F7357DFC7C96}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1406,7 +1406,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1F0270E-78F4-440C-92B7-47AD31428F28}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C82B33B-DA10-47A3-AAAB-7487BED83AF3}">
   <dimension ref="A1:AS125"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>